<commit_message>
Check in for December 28 Task
</commit_message>
<xml_diff>
--- a/modules/idaithalam/src/test/resources/Excels/virtualan_bdd_testcase_run_manager.xlsx
+++ b/modules/idaithalam/src/test/resources/Excels/virtualan_bdd_testcase_run_manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Extra\Final Test\idaithalam\modules\idaithalam\src\test\resources\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Extra\Conflict Resolving\idaithalam\modules\idaithalam\src\test\resources\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA964EA5-FC53-4DBB-B415-7E0CE65785BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3F0E5A-82D7-4D21-BA71-CE533D4A083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>code=MISSING_MOCK_DATA</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>pet</t>
   </si>
 </sst>
 </file>
@@ -500,160 +506,172 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G5" sqref="A5:XFD1450"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="176.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="205.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5546875" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" customWidth="1"/>
+    <col min="2" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="176.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="205.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5546875" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>200</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="282.60000000000002" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="H2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
+      <formula>LEN(TRIM(H2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>